<commit_message>
Reverted to commit 37a3b2bda1b45f920fb82a2ffea004dac9abffbd
</commit_message>
<xml_diff>
--- a/data_base_sistema.xlsx
+++ b/data_base_sistema.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c501bd79870a90b3/Área de Trabalho/GRUPO DOCTOR/git-push-fix/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c501bd79870a90b3/Área de Trabalho/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{7B6E4198-6283-462B-BCA9-B4B18471E882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CFB866E8-B231-4ECE-964C-34115DDA131C}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{7B6E4198-6283-462B-BCA9-B4B18471E882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63B9AC5B-E1EC-4609-9429-AE598F5C22BE}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CE004B1C-F3EA-4C30-AC9B-702894B35CAF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="9" activeTab="12" xr2:uid="{CE004B1C-F3EA-4C30-AC9B-702894B35CAF}"/>
   </bookViews>
   <sheets>
     <sheet name="00_empresas" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="199">
   <si>
     <t>id</t>
   </si>
@@ -633,15 +633,6 @@
   </si>
   <si>
     <t>I/VW PASSAT 2.0T FSI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cancelado </t>
-  </si>
-  <si>
-    <t>red</t>
-  </si>
-  <si>
-    <t>xis</t>
   </si>
 </sst>
 </file>
@@ -1186,10 +1177,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
@@ -1509,7 +1496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B7B662-3043-43D6-8E82-FB30A6D60723}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1664,7 +1651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E1FE9F-F3BB-43AC-B3F7-F37B752B57F2}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
@@ -2819,10 +2806,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6546B4F-78A8-45DA-A95A-26F3F6830D5D}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3024,26 +3011,6 @@
         <v>137</v>
       </c>
       <c r="F10" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>199</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>200</v>
-      </c>
-      <c r="D11" t="s">
-        <v>201</v>
-      </c>
-      <c r="E11" t="s">
-        <v>137</v>
-      </c>
-      <c r="F11" t="s">
         <v>163</v>
       </c>
     </row>

</xml_diff>